<commit_message>
Creación código completo API para todas las clases (API WIzard y modelo capas)
</commit_message>
<xml_diff>
--- a/Extenciones.xlsx
+++ b/Extenciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jafet\Desktop\ASADA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SC_701_ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{338B58B9-A681-4820-8797-F42B76444EEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC69E4C-5FF3-4E8C-8856-8BEFCDE5A213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{468FD89D-2680-4636-9B98-934E7B698109}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{468FD89D-2680-4636-9B98-934E7B698109}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -88,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -107,6 +107,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -196,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -205,6 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -223,7 +230,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -519,20 +526,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E558471-0CD6-4033-83C6-A8A77248F5FD}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -540,77 +547,86 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" s="8"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" s="8"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="8"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" s="8"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" s="8"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>